<commit_message>
Create Empty Object GameMaster that will instantiate the different objects in the environment within scripts. Did Timer count down and display the time in minutes and seconds.
</commit_message>
<xml_diff>
--- a/Wearables Game Mechanics.xlsx
+++ b/Wearables Game Mechanics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
   <si>
     <t xml:space="preserve">Clues are a part of the address for the structure with the hidden object; </t>
   </si>
@@ -265,6 +265,18 @@
   </si>
   <si>
     <t>Do they get any bonus points? Or how can they add some points?</t>
+  </si>
+  <si>
+    <t>Comments/Actions</t>
+  </si>
+  <si>
+    <t>Jul-16: Create a character and make it move arounf the world</t>
+  </si>
+  <si>
+    <t>Jul-17: Create timing display and PlayerStats class to count down time</t>
+  </si>
+  <si>
+    <t>Jul-17: Create PlayerStats class to manage score</t>
   </si>
 </sst>
 </file>
@@ -325,12 +337,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -394,12 +418,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -421,6 +447,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -439,28 +483,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -792,41 +831,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="79.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="62" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="21" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2"/>
@@ -907,16 +949,18 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2">
+      <c r="A12" s="22">
         <v>5</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="22" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
@@ -980,7 +1024,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="30">
       <c r="A19" s="2">
         <v>10</v>
       </c>
@@ -1026,7 +1070,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="30">
       <c r="A24" s="2">
         <v>12</v>
       </c>
@@ -1119,14 +1163,16 @@
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="2">
+      <c r="A34" s="22">
         <v>16</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
@@ -1138,7 +1184,7 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="30">
       <c r="A36" s="2">
         <v>18</v>
       </c>
@@ -1151,14 +1197,16 @@
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="2">
+      <c r="A37" s="22">
         <v>19</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="25" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2"/>
@@ -1168,11 +1216,11 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2"/>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="17"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2"/>
@@ -1264,7 +1312,7 @@
       </c>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" ht="30">
       <c r="A50" s="2">
         <v>25</v>
       </c>
@@ -1310,7 +1358,7 @@
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" ht="30">
       <c r="A55" s="2">
         <v>28</v>
       </c>
@@ -1320,7 +1368,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" ht="30">
       <c r="A56" s="2">
         <v>29</v>
       </c>
@@ -1402,11 +1450,11 @@
       <c r="A65" s="2">
         <v>33</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="20"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2"/>
@@ -1425,14 +1473,16 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="2">
+      <c r="A68" s="22">
         <v>34</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">

</xml_diff>

<commit_message>
Still working with Dangerous Zones shapefile. This is a project example with MapBox SDK for building city maps.
</commit_message>
<xml_diff>
--- a/Wearables Game Mechanics.xlsx
+++ b/Wearables Game Mechanics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t xml:space="preserve">Clues are a part of the address for the structure with the hidden object; </t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>Jul-17: Create PlayerStats class to manage score</t>
+  </si>
+  <si>
+    <t>Jul-17 Create TopSign and SideSigns Prefabs for this, but still not sure how the player will interact with them</t>
+  </si>
+  <si>
+    <t>Jul-16: Create a character and make it move around the world</t>
   </si>
 </sst>
 </file>
@@ -447,42 +453,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -493,6 +463,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -831,42 +837,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="62" style="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="9" t="s">
         <v>82</v>
       </c>
     </row>
@@ -949,17 +955,17 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="22">
+      <c r="A12" s="10">
         <v>5</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>83</v>
+      <c r="D12" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1162,19 +1168,19 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="22">
+    <row r="34" spans="1:4" ht="30">
+      <c r="A34" s="10">
         <v>16</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22" t="s">
+      <c r="C34" s="10"/>
+      <c r="D34" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="30">
       <c r="A35" s="2">
         <v>17</v>
       </c>
@@ -1185,26 +1191,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" ht="30">
-      <c r="A36" s="2">
+      <c r="A36" s="10">
         <v>18</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="13" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="22">
+      <c r="A37" s="10">
         <v>19</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="25" t="s">
+      <c r="C37" s="10"/>
+      <c r="D37" s="13" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1216,11 +1224,11 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2"/>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="11"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="16"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2"/>
@@ -1450,11 +1458,11 @@
       <c r="A65" s="2">
         <v>33</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="14"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="19"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2"/>
@@ -1473,14 +1481,14 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="22">
+      <c r="A68" s="10">
         <v>34</v>
       </c>
-      <c r="B68" s="23" t="s">
+      <c r="B68" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22" t="s">
+      <c r="C68" s="10"/>
+      <c r="D68" s="10" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1560,7 +1568,6 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>